<commit_message>
integração tela funcionários(em desenv)
</commit_message>
<xml_diff>
--- a/Cadastro de técnicos.xlsx
+++ b/Cadastro de técnicos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Nome" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CPF" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Telefone" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Turno" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="NomeEquipe" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nome" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CPF" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Telefone" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Turno" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NomeEquipe" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,9 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -454,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +472,9 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -480,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +501,9 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -506,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +530,9 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -532,7 +544,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,6 +559,9 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>